<commit_message>
Actualizacion cambio de envio de datos de REQUEST a POST
</commit_message>
<xml_diff>
--- a/pdf/tabla.xlsx
+++ b/pdf/tabla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/htdocs/cnt/LAIIProg/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8272B248-0A98-A444-AA3E-E08911DF85D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03ACEB1-AAF1-504A-BE81-D5BD74E060A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{84076746-44DA-4E99-A93B-BCEF9597C15B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{84076746-44DA-4E99-A93B-BCEF9597C15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7030,8 +7030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AA5ABD-FADB-4A1B-9A28-8EA690270BF2}">
   <dimension ref="A1:CP200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD97" zoomScale="200" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="CN102" sqref="CN102"/>
+    <sheetView tabSelected="1" topLeftCell="CJ94" zoomScale="200" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="CO104" sqref="CO104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12332,122 +12332,122 @@
       <c r="BC19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="BD19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BE19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BI19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BJ19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BP19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BQ19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BS19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BT19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BW19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BY19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BZ19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CC19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CD19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CF19" s="2" t="s">
-        <v>71</v>
+      <c r="BD19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BE19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BF19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BG19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BI19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BJ19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BK19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BL19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BM19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BN19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BP19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BQ19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BR19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BS19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BT19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BU19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BW19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BX19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BY19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BZ19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CA19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CB19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CC19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CD19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CE19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CF19" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="CG19" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="CH19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CI19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CJ19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CK19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CL19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CM19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CN19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CO19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CP19" s="2" t="s">
-        <v>71</v>
+      <c r="CH19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CI19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CJ19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CK19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CL19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CM19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CN19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CO19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="CP19" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:94" ht="17" x14ac:dyDescent="0.25">
@@ -35904,122 +35904,122 @@
       <c r="BC102" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="BD102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BE102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BI102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BJ102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BP102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BQ102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BS102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BT102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BW102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BY102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BZ102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CC102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CD102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CF102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CG102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CH102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CI102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CJ102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CK102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CL102" s="2" t="s">
-        <v>71</v>
+      <c r="BD102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BF102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BH102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BJ102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BN102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BP102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BQ102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BR102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BS102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BT102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BU102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BV102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BW102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BY102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="BZ102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CA102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CB102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CC102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CD102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CE102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CF102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CG102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CH102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CI102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CJ102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CK102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CL102" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="CM102" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="CN102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CO102" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CP102" s="2" t="s">
-        <v>71</v>
+      <c r="CN102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CO102" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="CP102" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:94" ht="17" x14ac:dyDescent="0.25">
@@ -37638,11 +37638,11 @@
       <c r="BM108" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BN108" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO108" s="4" t="s">
+      <c r="BN108" s="4" t="s">
         <v>245</v>
+      </c>
+      <c r="BO108" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="BP108" s="2" t="s">
         <v>71</v>

</xml_diff>